<commit_message>
Updating the tracker sheet for model training iterations
</commit_message>
<xml_diff>
--- a/Machine Learning Experiment Tracker.xlsx
+++ b/Machine Learning Experiment Tracker.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Garima\MS-DS\DTSA-5511 Introduction to Deep Learning\Finals\Santander Transaction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A4A1B9-812B-4FE3-9473-6D5C5D52ADD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61AAF4D-10ED-4F2D-88DB-2B1EA593BEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
-    <sheet name="Ideas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Title</t>
   </si>
@@ -44,63 +42,6 @@
   </si>
   <si>
     <t>Details</t>
-  </si>
-  <si>
-    <t>Idea</t>
-  </si>
-  <si>
-    <t>Potential Outcome</t>
-  </si>
-  <si>
-    <t>Learnings</t>
-  </si>
-  <si>
-    <t>Linear regression</t>
-  </si>
-  <si>
-    <t>Will be pretty bad</t>
-  </si>
-  <si>
-    <t>Ridge regression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">should be better than linear regression </t>
-  </si>
-  <si>
-    <t>Lasso regression</t>
-  </si>
-  <si>
-    <t>Polynomial regression</t>
-  </si>
-  <si>
-    <t>Decision Tree</t>
-  </si>
-  <si>
-    <t>Should offer good interpretation</t>
-  </si>
-  <si>
-    <t>Random Forests</t>
-  </si>
-  <si>
-    <t>Gradient Boosting</t>
-  </si>
-  <si>
-    <t>Support Vector Machine</t>
-  </si>
-  <si>
-    <t>Feature engineering</t>
-  </si>
-  <si>
-    <t>Improvmenet in accuracy</t>
-  </si>
-  <si>
-    <t>Increase max depth</t>
-  </si>
-  <si>
-    <t>Training loss &amp; validation loss go down</t>
-  </si>
-  <si>
-    <t>Try sample size 10%</t>
   </si>
   <si>
     <t>S No</t>
@@ -801,10 +742,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1074,31 +1014,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.609375" style="4"/>
+    <col min="1" max="1" width="12.609375" style="3"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20" style="4" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20" style="3" customWidth="1"/>
     <col min="6" max="6" width="43.94140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
-        <v>22</v>
+      <c r="A1" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1"/>
@@ -1121,21 +1061,21 @@
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="7">
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6">
         <v>0.86559600000000003</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="11" t="s">
-        <v>29</v>
+      <c r="E2" s="2"/>
+      <c r="F2" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1157,23 +1097,23 @@
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:24" ht="45.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="7">
+      <c r="B3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6">
         <v>0.89895899999999995</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>0.89634000000000003</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>52</v>
+      <c r="F3" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1195,392 +1135,264 @@
       <c r="X3" s="1"/>
     </row>
     <row r="4" spans="1:24" ht="45.3" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.89122999999999997</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.88958000000000004</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="51.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.89398999999999995</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.88983999999999996</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="51.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.89693000000000001</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.89537999999999995</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="46.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.89947999999999995</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0.89702999999999999</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="56.7" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.88892000000000004</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0.89149999999999996</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="63.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.89946000000000004</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0.90402000000000005</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="51.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.92135999999999996</v>
+      </c>
+      <c r="E10" s="12">
+        <v>0.91810000000000003</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="60.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.92248960000000002</v>
+      </c>
+      <c r="E11" s="12">
+        <v>0.91920000000000002</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.92217000000000005</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0.91961999999999999</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="56.7" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.92329300000000003</v>
+      </c>
+      <c r="E13" s="12">
+        <v>0.91966999999999999</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:24" ht="55.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.92090300000000003</v>
+      </c>
+      <c r="E14" s="12">
+        <v>0.91923999999999995</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="7">
-        <v>0.89122999999999997</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.88958000000000004</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="51.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="10" t="s">
+    </row>
+    <row r="15" spans="1:24" ht="59.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.92296</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0.92013999999999996</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="5">
-        <v>0.89398999999999995</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.88983999999999996</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" ht="51.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4">
+    </row>
+    <row r="16" spans="1:24" ht="49.2" x14ac:dyDescent="0.4">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="4">
-        <v>0.89693000000000001</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.89537999999999995</v>
-      </c>
-      <c r="F6" s="12" t="s">
+      <c r="D16" s="3">
+        <v>0.91829000000000005</v>
+      </c>
+      <c r="E16" s="12">
+        <v>0.91995000000000005</v>
+      </c>
+      <c r="F16" s="11" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" ht="46.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.89947999999999995</v>
-      </c>
-      <c r="E7" s="13">
-        <v>0.89702999999999999</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="56.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.88892000000000004</v>
-      </c>
-      <c r="E8" s="13">
-        <v>0.89149999999999996</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" ht="63.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0.89946000000000004</v>
-      </c>
-      <c r="E9" s="13">
-        <v>0.90402000000000005</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="51.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.92135999999999996</v>
-      </c>
-      <c r="E10" s="13">
-        <v>0.91810000000000003</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" ht="60.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.92248960000000002</v>
-      </c>
-      <c r="E11" s="13">
-        <v>0.91920000000000002</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0.92217000000000005</v>
-      </c>
-      <c r="E12" s="13">
-        <v>0.91961999999999999</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" ht="56.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.92329300000000003</v>
-      </c>
-      <c r="E13" s="13">
-        <v>0.91966999999999999</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="1:24" ht="55.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.92090300000000003</v>
-      </c>
-      <c r="E14" s="13">
-        <v>0.91923999999999995</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" ht="59.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.92296</v>
-      </c>
-      <c r="E15" s="15">
-        <v>0.92013999999999996</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" ht="49.2" x14ac:dyDescent="0.4">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0.91829000000000005</v>
-      </c>
-      <c r="E16" s="13">
-        <v>0.91995000000000005</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:Z14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="43.609375" customWidth="1"/>
-    <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="54.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>